<commit_message>
Broke off global namespace. Renamed Range.values -> Range.value.
</commit_message>
<xml_diff>
--- a/examples/ranges/out.xlsx
+++ b/examples/ranges/out.xlsx
@@ -1732,10 +1732,10 @@
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3"/>
       <c r="B3" s="1">
-        <v>120</v>
+        <v>590</v>
       </c>
       <c r="C3" s="1">
-        <v>537206</v>
+        <v>614036</v>
       </c>
       <c r="D3" s="5">
         <f t="shared" si="1" ref="D3:D13">B3/C3</f>
@@ -1744,10 +1744,10 @@
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4"/>
       <c r="B4" s="1">
-        <v>963</v>
+        <v>795</v>
       </c>
       <c r="C4" s="1">
-        <v>709012</v>
+        <v>200127</v>
       </c>
       <c r="D4" s="6">
         <f t="shared" si="1"/>
@@ -1756,10 +1756,10 @@
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5"/>
       <c r="B5" s="1">
-        <v>5</v>
+        <v>858</v>
       </c>
       <c r="C5" s="1">
-        <v>108734</v>
+        <v>341388</v>
       </c>
       <c r="D5" s="7">
         <f t="shared" si="1"/>
@@ -1768,10 +1768,10 @@
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6"/>
       <c r="B6">
-        <v>133</v>
+        <v>849</v>
       </c>
       <c r="C6" s="1">
-        <v>176391</v>
+        <v>408012</v>
       </c>
       <c r="D6" s="8">
         <f t="shared" si="1"/>
@@ -1780,10 +1780,10 @@
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7"/>
       <c r="B7" s="1">
-        <v>331</v>
+        <v>892</v>
       </c>
       <c r="C7" s="1">
-        <v>540508</v>
+        <v>202438</v>
       </c>
       <c r="D7" s="9">
         <f t="shared" si="1"/>
@@ -1792,10 +1792,10 @@
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8"/>
       <c r="B8">
-        <v>772</v>
+        <v>847</v>
       </c>
       <c r="C8" s="1">
-        <v>515482</v>
+        <v>811081</v>
       </c>
       <c r="D8" s="10">
         <f t="shared" si="1"/>
@@ -1804,10 +1804,10 @@
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9"/>
       <c r="B9">
-        <v>821</v>
+        <v>391</v>
       </c>
       <c r="C9" s="1">
-        <v>913074</v>
+        <v>377913</v>
       </c>
       <c r="D9" s="11">
         <f t="shared" si="1"/>
@@ -1816,10 +1816,10 @@
     <row r="10">
       <c r="A10"/>
       <c r="B10">
-        <v>613</v>
+        <v>854</v>
       </c>
       <c r="C10">
-        <v>586719</v>
+        <v>157944</v>
       </c>
       <c r="D10" s="12">
         <f t="shared" si="1"/>
@@ -1828,10 +1828,10 @@
     <row r="11">
       <c r="A11"/>
       <c r="B11">
-        <v>726</v>
+        <v>643</v>
       </c>
       <c r="C11">
-        <v>5222</v>
+        <v>877947</v>
       </c>
       <c r="D11" s="13">
         <f t="shared" si="1"/>
@@ -1840,10 +1840,10 @@
     <row r="12">
       <c r="A12"/>
       <c r="B12">
-        <v>434</v>
+        <v>378</v>
       </c>
       <c r="C12">
-        <v>981949</v>
+        <v>388269</v>
       </c>
       <c r="D12" s="14">
         <f t="shared" si="1"/>
@@ -1852,10 +1852,10 @@
     <row r="13">
       <c r="A13"/>
       <c r="B13">
-        <v>909</v>
+        <v>643</v>
       </c>
       <c r="C13">
-        <v>462860</v>
+        <v>747905</v>
       </c>
       <c r="D13" s="15">
         <f t="shared" si="1"/>

</xml_diff>

<commit_message>
Shaved memory a bit and removed xmlbuilder.
</commit_message>
<xml_diff>
--- a/examples/ranges/out.xlsx
+++ b/examples/ranges/out.xlsx
@@ -1732,10 +1732,10 @@
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3"/>
       <c r="B3" s="1">
-        <v>590</v>
+        <v>829</v>
       </c>
       <c r="C3" s="1">
-        <v>614036</v>
+        <v>381284</v>
       </c>
       <c r="D3" s="5">
         <f t="shared" si="1" ref="D3:D13">B3/C3</f>
@@ -1744,10 +1744,10 @@
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4"/>
       <c r="B4" s="1">
-        <v>795</v>
+        <v>447</v>
       </c>
       <c r="C4" s="1">
-        <v>200127</v>
+        <v>6948</v>
       </c>
       <c r="D4" s="6">
         <f t="shared" si="1"/>
@@ -1756,10 +1756,10 @@
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5"/>
       <c r="B5" s="1">
-        <v>858</v>
+        <v>994</v>
       </c>
       <c r="C5" s="1">
-        <v>341388</v>
+        <v>500248</v>
       </c>
       <c r="D5" s="7">
         <f t="shared" si="1"/>
@@ -1768,10 +1768,10 @@
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6"/>
       <c r="B6">
-        <v>849</v>
+        <v>991</v>
       </c>
       <c r="C6" s="1">
-        <v>408012</v>
+        <v>203884</v>
       </c>
       <c r="D6" s="8">
         <f t="shared" si="1"/>
@@ -1780,10 +1780,10 @@
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7"/>
       <c r="B7" s="1">
-        <v>892</v>
+        <v>385</v>
       </c>
       <c r="C7" s="1">
-        <v>202438</v>
+        <v>11742</v>
       </c>
       <c r="D7" s="9">
         <f t="shared" si="1"/>
@@ -1792,10 +1792,10 @@
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8"/>
       <c r="B8">
-        <v>847</v>
+        <v>102</v>
       </c>
       <c r="C8" s="1">
-        <v>811081</v>
+        <v>733063</v>
       </c>
       <c r="D8" s="10">
         <f t="shared" si="1"/>
@@ -1804,10 +1804,10 @@
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9"/>
       <c r="B9">
-        <v>391</v>
+        <v>557</v>
       </c>
       <c r="C9" s="1">
-        <v>377913</v>
+        <v>603286</v>
       </c>
       <c r="D9" s="11">
         <f t="shared" si="1"/>
@@ -1816,10 +1816,10 @@
     <row r="10">
       <c r="A10"/>
       <c r="B10">
-        <v>854</v>
+        <v>319</v>
       </c>
       <c r="C10">
-        <v>157944</v>
+        <v>34247</v>
       </c>
       <c r="D10" s="12">
         <f t="shared" si="1"/>
@@ -1828,10 +1828,10 @@
     <row r="11">
       <c r="A11"/>
       <c r="B11">
-        <v>643</v>
+        <v>58</v>
       </c>
       <c r="C11">
-        <v>877947</v>
+        <v>666750</v>
       </c>
       <c r="D11" s="13">
         <f t="shared" si="1"/>
@@ -1840,10 +1840,10 @@
     <row r="12">
       <c r="A12"/>
       <c r="B12">
-        <v>378</v>
+        <v>335</v>
       </c>
       <c r="C12">
-        <v>388269</v>
+        <v>123792</v>
       </c>
       <c r="D12" s="14">
         <f t="shared" si="1"/>
@@ -1852,10 +1852,10 @@
     <row r="13">
       <c r="A13"/>
       <c r="B13">
-        <v>643</v>
+        <v>389</v>
       </c>
       <c r="C13">
-        <v>747905</v>
+        <v>348994</v>
       </c>
       <c r="D13" s="15">
         <f t="shared" si="1"/>

</xml_diff>

<commit_message>
Fixed shared strings bug, whitespace handlnig, XML escaping, and workbook race condition.
</commit_message>
<xml_diff>
--- a/examples/ranges/out.xlsx
+++ b/examples/ranges/out.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <si>
     <t>Clicks</t>
   </si>
@@ -1732,10 +1732,10 @@
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3"/>
       <c r="B3" s="1">
-        <v>829</v>
+        <v>937</v>
       </c>
       <c r="C3" s="1">
-        <v>381284</v>
+        <v>965560</v>
       </c>
       <c r="D3" s="5">
         <f t="shared" si="1" ref="D3:D13">B3/C3</f>
@@ -1744,10 +1744,10 @@
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4"/>
       <c r="B4" s="1">
-        <v>447</v>
+        <v>120</v>
       </c>
       <c r="C4" s="1">
-        <v>6948</v>
+        <v>361403</v>
       </c>
       <c r="D4" s="6">
         <f t="shared" si="1"/>
@@ -1756,10 +1756,10 @@
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5"/>
       <c r="B5" s="1">
-        <v>994</v>
+        <v>561</v>
       </c>
       <c r="C5" s="1">
-        <v>500248</v>
+        <v>154880</v>
       </c>
       <c r="D5" s="7">
         <f t="shared" si="1"/>
@@ -1768,10 +1768,10 @@
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6"/>
       <c r="B6">
-        <v>991</v>
+        <v>554</v>
       </c>
       <c r="C6" s="1">
-        <v>203884</v>
+        <v>506691</v>
       </c>
       <c r="D6" s="8">
         <f t="shared" si="1"/>
@@ -1780,10 +1780,10 @@
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7"/>
       <c r="B7" s="1">
-        <v>385</v>
+        <v>451</v>
       </c>
       <c r="C7" s="1">
-        <v>11742</v>
+        <v>201358</v>
       </c>
       <c r="D7" s="9">
         <f t="shared" si="1"/>
@@ -1792,10 +1792,10 @@
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8"/>
       <c r="B8">
-        <v>102</v>
+        <v>80</v>
       </c>
       <c r="C8" s="1">
-        <v>733063</v>
+        <v>273339</v>
       </c>
       <c r="D8" s="10">
         <f t="shared" si="1"/>
@@ -1804,10 +1804,10 @@
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9"/>
       <c r="B9">
-        <v>557</v>
+        <v>146</v>
       </c>
       <c r="C9" s="1">
-        <v>603286</v>
+        <v>901638</v>
       </c>
       <c r="D9" s="11">
         <f t="shared" si="1"/>
@@ -1816,10 +1816,10 @@
     <row r="10">
       <c r="A10"/>
       <c r="B10">
-        <v>319</v>
+        <v>853</v>
       </c>
       <c r="C10">
-        <v>34247</v>
+        <v>889534</v>
       </c>
       <c r="D10" s="12">
         <f t="shared" si="1"/>
@@ -1828,10 +1828,10 @@
     <row r="11">
       <c r="A11"/>
       <c r="B11">
-        <v>58</v>
+        <v>995</v>
       </c>
       <c r="C11">
-        <v>666750</v>
+        <v>735120</v>
       </c>
       <c r="D11" s="13">
         <f t="shared" si="1"/>
@@ -1840,10 +1840,10 @@
     <row r="12">
       <c r="A12"/>
       <c r="B12">
-        <v>335</v>
+        <v>373</v>
       </c>
       <c r="C12">
-        <v>123792</v>
+        <v>995785</v>
       </c>
       <c r="D12" s="14">
         <f t="shared" si="1"/>
@@ -1852,10 +1852,10 @@
     <row r="13">
       <c r="A13"/>
       <c r="B13">
-        <v>389</v>
+        <v>254</v>
       </c>
       <c r="C13">
-        <v>348994</v>
+        <v>727259</v>
       </c>
       <c r="D13" s="15">
         <f t="shared" si="1"/>

</xml_diff>